<commit_message>
Table 1 domain analysis corrected
</commit_message>
<xml_diff>
--- a/table1.xlsx
+++ b/table1.xlsx
@@ -211,9 +211,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AAA1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -260,25 +260,25 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>2.629e+003</v>
+        <v>2629</v>
       </c>
       <c r="C2">
-        <v>1.2486114311188578e-001</v>
+        <v>.12486114311188569</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2">
-        <v>5.02e+002</v>
+        <v>502</v>
       </c>
       <c r="F2">
-        <v>4.3274066904212472e-001</v>
+        <v>.18507942308033346</v>
       </c>
       <c r="G2">
-        <v>1.185e+003</v>
+        <v>1185</v>
       </c>
       <c r="H2">
-        <v>1.6353579652259004e-001</v>
+        <v>.4898956146358516</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -286,25 +286,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>3.135e+003</v>
+        <v>3135</v>
       </c>
       <c r="C3">
-        <v>2.625538670717636e-001</v>
+        <v>.26255386707176337</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>3.19e+002</v>
+        <v>319</v>
       </c>
       <c r="F3">
-        <v>4.7693075157477456e-001</v>
+        <v>.0797996404560808</v>
       </c>
       <c r="G3">
-        <v>1.419e+003</v>
+        <v>1419</v>
       </c>
       <c r="H3">
-        <v>7.6923429205652576e-002</v>
+        <v>.495217650639752</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -312,25 +312,25 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>3.84e+003</v>
+        <v>3840</v>
       </c>
       <c r="C4">
-        <v>2.4490627733231408e-001</v>
+        <v>.24490627733231402</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4">
-        <v>6.72e+002</v>
+        <v>672</v>
       </c>
       <c r="F4">
-        <v>2.6189816929697756e-001</v>
+        <v>.15581981197122155</v>
       </c>
       <c r="G4">
-        <v>1.83e+003</v>
+        <v>1830</v>
       </c>
       <c r="H4">
-        <v>7.7853288514700256e-002</v>
+        <v>.5244569490000929</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -338,25 +338,25 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2.059e+003</v>
+        <v>2059</v>
       </c>
       <c r="C5">
-        <v>6.598153257734976e-002</v>
+        <v>.06598153257734969</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5">
-        <v>3.56e+002</v>
+        <v>356</v>
       </c>
       <c r="F5">
-        <v>9.382765525337384e-001</v>
+        <v>.16169120180728133</v>
       </c>
       <c r="G5">
-        <v>8.41e+002</v>
+        <v>841</v>
       </c>
       <c r="H5">
-        <v>3.513613290731906e-001</v>
+        <v>.43136326543532655</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -364,25 +364,25 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>4.382e+003</v>
+        <v>4382</v>
       </c>
       <c r="C6">
-        <v>3.0169717990668756e-001</v>
+        <v>.30169717990668726</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6">
-        <v>7.39e+002</v>
+        <v>739</v>
       </c>
       <c r="F6">
-        <v>2.2278046231375272e-001</v>
+        <v>.14891291937343276</v>
       </c>
       <c r="G6">
-        <v>2.04e+003</v>
+        <v>2040</v>
       </c>
       <c r="H6">
-        <v>6.4637022887462096e-002</v>
+        <v>.5126616125361327</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -390,25 +390,25 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>8.073e+003</v>
+        <v>8073</v>
       </c>
       <c r="C7">
-        <v>5.1176271206351008e-001</v>
+        <v>.5117627120635093</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7">
-        <v>1.297e+003</v>
+        <v>1297</v>
       </c>
       <c r="F7">
-        <v>1.442547675554102e-001</v>
+        <v>.1354983682157096</v>
       </c>
       <c r="G7">
-        <v>3.84e+003</v>
+        <v>3840</v>
       </c>
       <c r="H7">
-        <v>3.731206603471576e-002</v>
+        <v>.523752820413486</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -416,25 +416,25 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>7.999e+003</v>
+        <v>7999</v>
       </c>
       <c r="C8">
-        <v>4.882372879364908e-001</v>
+        <v>.4882372879364906</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8">
-        <v>1.296e+003</v>
+        <v>1296</v>
       </c>
       <c r="F8">
-        <v>1.4555300154929786e-001</v>
+        <v>.140672320312189</v>
       </c>
       <c r="G8">
-        <v>3.482e+003</v>
+        <v>3482</v>
       </c>
       <c r="H8">
-        <v>4.2651344716308e-002</v>
+        <v>.48016432037236295</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -442,25 +442,25 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>2.895e+003</v>
+        <v>2895</v>
       </c>
       <c r="C9">
-        <v>8.1401054607111872e-002</v>
+        <v>.08140105460711192</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9">
-        <v>3.77e+002</v>
+        <v>377</v>
       </c>
       <c r="F9">
-        <v>1.0132250682125768e+000</v>
+        <v>.12119582655744879</v>
       </c>
       <c r="G9">
-        <v>1.166e+003</v>
+        <v>1166</v>
       </c>
       <c r="H9">
-        <v>2.976045460555092e-001</v>
+        <v>.41280301368474204</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -468,25 +468,25 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>3.295e+003</v>
+        <v>3295</v>
       </c>
       <c r="C10">
-        <v>1.133998269045961e-001</v>
+        <v>.11339982690459612</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10">
-        <v>8.51e+002</v>
+        <v>851</v>
       </c>
       <c r="F10">
-        <v>3.3446088309818072e-001</v>
+        <v>.263793461420665</v>
       </c>
       <c r="G10">
-        <v>1.527e+003</v>
+        <v>1527</v>
       </c>
       <c r="H10">
-        <v>1.8993898200570412e-001</v>
+        <v>.4641894244684604</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -494,25 +494,25 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>7.779e+003</v>
+        <v>7779</v>
       </c>
       <c r="C11">
-        <v>6.9979050263761856e-001</v>
+        <v>.6997905026376184</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11">
-        <v>9.87e+002</v>
+        <v>987</v>
       </c>
       <c r="F11">
-        <v>1.2363546706212772e-001</v>
+        <v>.11557434011829944</v>
       </c>
       <c r="G11">
-        <v>3.817e+003</v>
+        <v>3817</v>
       </c>
       <c r="H11">
-        <v>2.699818511913054e-002</v>
+        <v>.529225081865937</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,25 +520,25 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>1.371e+003</v>
+        <v>1371</v>
       </c>
       <c r="C12">
-        <v>4.4311190171690096e-002</v>
+        <v>.04431119017169008</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
       <c r="E12">
-        <v>2.46e+002</v>
+        <v>246</v>
       </c>
       <c r="F12">
-        <v>1.3878321047044872e+000</v>
+        <v>.1624588145847037</v>
       </c>
       <c r="G12">
-        <v>5.19e+002</v>
+        <v>519</v>
       </c>
       <c r="H12">
-        <v>5.4130305462876208e-001</v>
+        <v>.4167798661601008</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -546,25 +546,25 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>7.32e+002</v>
+        <v>732</v>
       </c>
       <c r="C13">
-        <v>6.1097425678983344e-002</v>
+        <v>.06109742567898335</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
       <c r="E13">
-        <v>1.32e+002</v>
+        <v>132</v>
       </c>
       <c r="F13">
-        <v>9.8342588947265936e-001</v>
+        <v>.16659755285831082</v>
       </c>
       <c r="G13">
-        <v>2.93e+002</v>
+        <v>293</v>
       </c>
       <c r="H13">
-        <v>3.6563496248657408e-001</v>
+        <v>.448551759142935</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -572,25 +572,25 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>1.004e+003</v>
+        <v>1004</v>
       </c>
       <c r="C14">
-        <v>5.7478270001196488e-002</v>
+        <v>.05747827000119642</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
       <c r="E14">
-        <v>1.92e+002</v>
+        <v>192</v>
       </c>
       <c r="F14">
-        <v>1.0407092205182976e+000</v>
+        <v>.16712454268678914</v>
       </c>
       <c r="G14">
-        <v>3.89e+002</v>
+        <v>389</v>
       </c>
       <c r="H14">
-        <v>4.0853161778256472e-001</v>
+        <v>.4261183170491705</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -598,25 +598,25 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>7.999e+003</v>
+        <v>7999</v>
       </c>
       <c r="C15">
-        <v>4.8823728793649104e-001</v>
+        <v>.4882372879364907</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
       <c r="E15">
-        <v>1.296e+003</v>
+        <v>1296</v>
       </c>
       <c r="F15">
-        <v>1.4555300154929786e-001</v>
+        <v>.140672320312189</v>
       </c>
       <c r="G15">
-        <v>3.482e+003</v>
+        <v>3482</v>
       </c>
       <c r="H15">
-        <v>4.2651344716308e-002</v>
+        <v>.48016432037236295</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -624,25 +624,25 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>6.545e+003</v>
+        <v>6545</v>
       </c>
       <c r="C16">
-        <v>4.1109090558527344e-001</v>
+        <v>.4110909055852731</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
       <c r="E16">
-        <v>1.037e+003</v>
+        <v>1037</v>
       </c>
       <c r="F16">
-        <v>1.8136941785547412e-001</v>
+        <v>.13419117579856057</v>
       </c>
       <c r="G16">
-        <v>3.188e+003</v>
+        <v>3188</v>
       </c>
       <c r="H16">
-        <v>4.5845925676703912e-002</v>
+        <v>.5306338017094295</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -650,25 +650,25 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>5.24e+002</v>
+        <v>524</v>
       </c>
       <c r="C17">
-        <v>4.3193536477039944e-002</v>
+        <v>.04319353647703991</v>
       </c>
       <c r="D17" t="s">
         <v>27</v>
       </c>
       <c r="E17">
-        <v>6.8e+001</v>
+        <v>68</v>
       </c>
       <c r="F17">
-        <v>2.184894484280756e+000</v>
+        <v>.10586304778593553</v>
       </c>
       <c r="G17">
-        <v>2.63e+002</v>
+        <v>263</v>
       </c>
       <c r="H17">
-        <v>3.9354558844858496e-001</v>
+        <v>.5880940858461586</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,25 +676,25 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>4.191e+003</v>
+        <v>4191</v>
       </c>
       <c r="C18">
-        <v>2.668761193923872e-001</v>
+        <v>.2668761193923869</v>
       </c>
       <c r="D18" t="s">
         <v>29</v>
       </c>
       <c r="E18">
-        <v>8.4e+002</v>
+        <v>840</v>
       </c>
       <c r="F18">
-        <v>2.0083704085559472e-001</v>
+        <v>.1867148477516125</v>
       </c>
       <c r="G18">
-        <v>2.022e+003</v>
+        <v>2022</v>
       </c>
       <c r="H18">
-        <v>7.069843037713252e-002</v>
+        <v>.5299426217271924</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -702,25 +702,25 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>1.1881e+004</v>
+        <v>11881</v>
       </c>
       <c r="C19">
-        <v>7.3312388060761344e-001</v>
+        <v>.7331238806076127</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
       </c>
       <c r="E19">
-        <v>1.753e+003</v>
+        <v>1753</v>
       </c>
       <c r="F19">
-        <v>1.1333540321422844e-001</v>
+        <v>.12031952446696824</v>
       </c>
       <c r="G19">
-        <v>5.3e+003</v>
+        <v>5300</v>
       </c>
       <c r="H19">
-        <v>2.7699054178133496e-002</v>
+        <v>.4924662840631326</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -728,25 +728,25 @@
         <v>31</v>
       </c>
       <c r="B20">
-        <v>1.191e+003</v>
+        <v>1191</v>
       </c>
       <c r="C20">
-        <v>7.1414271567199952e-002</v>
+        <v>.07141427156719986</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
       <c r="E20">
-        <v>2.12e+002</v>
+        <v>212</v>
       </c>
       <c r="F20">
-        <v>8.8522980032501216e-001</v>
+        <v>.15811668149210137</v>
       </c>
       <c r="G20">
-        <v>4.86e+002</v>
+        <v>486</v>
       </c>
       <c r="H20">
-        <v>3.0886441929042528e-001</v>
+        <v>.4535537831821629</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,25 +754,25 @@
         <v>31</v>
       </c>
       <c r="B21">
-        <v>7.999e+003</v>
+        <v>7999</v>
       </c>
       <c r="C21">
-        <v>4.8823728793649112e-001</v>
+        <v>.4882372879364907</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
       <c r="E21">
-        <v>1.296e+003</v>
+        <v>1296</v>
       </c>
       <c r="F21">
-        <v>1.4555300154929788e-001</v>
+        <v>.140672320312189</v>
       </c>
       <c r="G21">
-        <v>3.482e+003</v>
+        <v>3482</v>
       </c>
       <c r="H21">
-        <v>4.2651344716308e-002</v>
+        <v>.48016432037236295</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -780,25 +780,25 @@
         <v>31</v>
       </c>
       <c r="B22">
-        <v>6.616e+003</v>
+        <v>6616</v>
       </c>
       <c r="C22">
-        <v>4.1965335651746504e-001</v>
+        <v>.4196533565174644</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
       </c>
       <c r="E22">
-        <v>1.053e+003</v>
+        <v>1053</v>
       </c>
       <c r="F22">
-        <v>1.782043372168967e-001</v>
+        <v>.1337839473476835</v>
       </c>
       <c r="G22">
-        <v>3.19e+003</v>
+        <v>3190</v>
       </c>
       <c r="H22">
-        <v>4.5028947847968128e-002</v>
+        <v>.5292337080994438</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,25 +806,25 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>2.66e+002</v>
+        <v>266</v>
       </c>
       <c r="C23">
-        <v>2.0695083978845288e-002</v>
+        <v>.02069508397884525</v>
       </c>
       <c r="D23" t="s">
         <v>27</v>
       </c>
       <c r="E23">
-        <v>3.2e+001</v>
+        <v>32</v>
       </c>
       <c r="F23">
-        <v>5.2357659140491192e+000</v>
+        <v>.0922032459515263</v>
       </c>
       <c r="G23">
-        <v>1.64e+002</v>
+        <v>164</v>
       </c>
       <c r="H23">
-        <v>7.3780101647091808e-001</v>
+        <v>.6547178499619064</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -832,25 +832,25 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>1.0262e+004</v>
+        <v>10262</v>
       </c>
       <c r="C24">
-        <v>6.5871127222261144e-001</v>
+        <v>.6587112722226114</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
       </c>
       <c r="E24">
-        <v>1.499e+003</v>
+        <v>1499</v>
       </c>
       <c r="F24">
-        <v>1.2031148178383044e-001</v>
+        <v>.1261754722221648</v>
       </c>
       <c r="G24">
-        <v>4.702e+003</v>
+        <v>4702</v>
       </c>
       <c r="H24">
-        <v>2.9928217895383564e-002</v>
+        <v>.5072758279664283</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -858,25 +858,25 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>5.81e+003</v>
+        <v>5810</v>
       </c>
       <c r="C25">
-        <v>3.4128872777738872e-001</v>
+        <v>.3412887277773887</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
       </c>
       <c r="E25">
-        <v>1.094e+003</v>
+        <v>1094</v>
       </c>
       <c r="F25">
-        <v>1.82123792058329e-001</v>
+        <v>.1608998184941224</v>
       </c>
       <c r="G25">
-        <v>2.62e+003</v>
+        <v>2620</v>
       </c>
       <c r="H25">
-        <v>5.9404933093248552e-002</v>
+        <v>.49319278243276726</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -884,25 +884,25 @@
         <v>41</v>
       </c>
       <c r="B26">
-        <v>4.442e+003</v>
+        <v>4442</v>
       </c>
       <c r="C26">
-        <v>3.2367441707480756e-001</v>
+        <v>.3236744170748077</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26">
-        <v>6.95e+002</v>
+        <v>695</v>
       </c>
       <c r="F26">
-        <v>2.2935218210166776e-001</v>
+        <v>.13479304388939517</v>
       </c>
       <c r="G26">
-        <v>3.27e+003</v>
+        <v>3270</v>
       </c>
       <c r="H26">
-        <v>4.0157408872900072e-002</v>
+        <v>.7692280837800479</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -910,25 +910,25 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <v>3.409e+003</v>
+        <v>3409</v>
       </c>
       <c r="C27">
-        <v>1.5919464430513562e-001</v>
+        <v>.15919464430513572</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
       </c>
       <c r="E27">
-        <v>5.94e+002</v>
+        <v>594</v>
       </c>
       <c r="F27">
-        <v>4.0682157851254424e-001</v>
+        <v>.15434045425639598</v>
       </c>
       <c r="G27">
-        <v>1.188e+003</v>
+        <v>1188</v>
       </c>
       <c r="H27">
-        <v>1.7506449514044788e-001</v>
+        <v>.35881286903998816</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -936,25 +936,25 @@
         <v>41</v>
       </c>
       <c r="B28">
-        <v>8.221e+003</v>
+        <v>8221</v>
       </c>
       <c r="C28">
-        <v>5.1713093862005616e-001</v>
+        <v>.5171309386200567</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
       </c>
       <c r="E28">
-        <v>1.304e+003</v>
+        <v>1304</v>
       </c>
       <c r="F28">
-        <v>1.431773967150543e-001</v>
+        <v>.13502321735951536</v>
       </c>
       <c r="G28">
-        <v>2.864e+003</v>
+        <v>2864</v>
       </c>
       <c r="H28">
-        <v>5.0935388328345e-002</v>
+        <v>.3796871203729662</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -962,25 +962,25 @@
         <v>34</v>
       </c>
       <c r="B29">
-        <v>4.316e+003</v>
+        <v>4316</v>
       </c>
       <c r="C29">
-        <v>1.8972914844892752e-001</v>
+        <v>.1897291484489276</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
       </c>
       <c r="E29">
-        <v>8.39e+002</v>
+        <v>839</v>
       </c>
       <c r="F29">
-        <v>2.8186311462383356e-001</v>
+        <v>.1872257421535215</v>
       </c>
       <c r="G29">
-        <v>1.778e+003</v>
+        <v>1778</v>
       </c>
       <c r="H29">
-        <v>1.158921091444377e-001</v>
+        <v>.45477657312446507</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -988,25 +988,25 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>3.962e+003</v>
+        <v>3962</v>
       </c>
       <c r="C30">
-        <v>1.8997926591229688e-001</v>
+        <v>.18997926591229702</v>
       </c>
       <c r="D30" t="s">
         <v>36</v>
       </c>
       <c r="E30">
-        <v>6.83e+002</v>
+        <v>683</v>
       </c>
       <c r="F30">
-        <v>3.114943605136068e-001</v>
+        <v>.1691324883782244</v>
       </c>
       <c r="G30">
-        <v>1.794e+003</v>
+        <v>1794</v>
       </c>
       <c r="H30">
-        <v>1.037529368190445e-001</v>
+        <v>.5074442518790123</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1014,25 +1014,25 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>7.794e+003</v>
+        <v>7794</v>
       </c>
       <c r="C31">
-        <v>6.2029158563877488e-001</v>
+        <v>.6202915856387755</v>
       </c>
       <c r="D31" t="s">
         <v>37</v>
       </c>
       <c r="E31">
-        <v>1.071e+003</v>
+        <v>1071</v>
       </c>
       <c r="F31">
-        <v>1.4195719450661228e-001</v>
+        <v>.1134919334581784</v>
       </c>
       <c r="G31">
-        <v>3.75e+003</v>
+        <v>3750</v>
       </c>
       <c r="H31">
-        <v>3.1269636557201928e-002</v>
+        <v>.5155330137327362</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,19 +1040,19 @@
         <v>38</v>
       </c>
       <c r="B32">
-        <v>8.741e+003</v>
+        <v>8741</v>
       </c>
       <c r="C32">
-        <v>4.9753098650550064e-001</v>
+        <v>.4975309865055008</v>
       </c>
       <c r="D32" t="s">
         <v>26</v>
       </c>
       <c r="E32">
-        <v>1.143e+003</v>
+        <v>1143</v>
       </c>
       <c r="F32">
-        <v>1.8571772250622728e-001</v>
+        <v>.10819496651045324</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1060,19 +1060,19 @@
         <v>38</v>
       </c>
       <c r="B33">
-        <v>7.322e+003</v>
+        <v>7322</v>
       </c>
       <c r="C33">
-        <v>5.0246901349449936e-001</v>
+        <v>.5024690134944994</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
       </c>
       <c r="E33">
-        <v>1.448e+003</v>
+        <v>1448</v>
       </c>
       <c r="F33">
-        <v>1.189148184844568e-001</v>
+        <v>.1674067851789359</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1080,19 +1080,19 @@
         <v>39</v>
       </c>
       <c r="B34">
-        <v>1.346e+004</v>
+        <v>13460</v>
       </c>
       <c r="C34">
-        <v>8.6197470541915648e-001</v>
+        <v>.8619747054191564</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
       </c>
       <c r="G34">
-        <v>5.862e+003</v>
+        <v>5862</v>
       </c>
       <c r="H34">
-        <v>2.3909812280776208e-002</v>
+        <v>.48516092861343796</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1100,19 +1100,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>2.593e+003</v>
+        <v>2593</v>
       </c>
       <c r="C35">
-        <v>1.3802529458084356e-001</v>
+        <v>.13802529458084364</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
       </c>
       <c r="G35">
-        <v>1.448e+003</v>
+        <v>1448</v>
       </c>
       <c r="H35">
-        <v>1.189148184844568e-001</v>
+        <v>.6096450559820747</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1120,25 +1120,25 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>6.12e+002</v>
+        <v>612</v>
       </c>
       <c r="C36">
-        <v>4.055348062536868e-002</v>
+        <v>.04055348062536871</v>
       </c>
       <c r="D36" t="s">
         <v>24</v>
       </c>
       <c r="E36">
-        <v>1.53e+002</v>
+        <v>153</v>
       </c>
       <c r="F36">
-        <v>1.1499444556588044e+000</v>
+        <v>.21491655551873742</v>
       </c>
       <c r="G36">
-        <v>5.48e+002</v>
+        <v>548</v>
       </c>
       <c r="H36">
-        <v>2.7267546982870032e-001</v>
+        <v>.9046874261574475</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1146,25 +1146,25 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>1.4659e+004</v>
+        <v>14659</v>
       </c>
       <c r="C37">
-        <v>9.0202366472776176e-001</v>
+        <v>.9020236647277617</v>
       </c>
       <c r="D37" t="s">
         <v>26</v>
       </c>
       <c r="E37">
-        <v>2.246e+003</v>
+        <v>2246</v>
       </c>
       <c r="F37">
-        <v>8.5412835496502944e-002</v>
+        <v>.12978994006035618</v>
       </c>
       <c r="G37">
-        <v>6.013e+003</v>
+        <v>6013</v>
       </c>
       <c r="H37">
-        <v>2.4353134544644168e-002</v>
+        <v>.4552273107625041</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1172,25 +1172,25 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>8.01e+002</v>
+        <v>801</v>
       </c>
       <c r="C38">
-        <v>5.7422854646869056e-002</v>
+        <v>.057422854646869116</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
       </c>
       <c r="E38">
-        <v>1.94e+002</v>
+        <v>194</v>
       </c>
       <c r="F38">
-        <v>8.1627319806786528e-001</v>
+        <v>.21314409695001446</v>
       </c>
       <c r="G38">
-        <v>7.61e+002</v>
+        <v>761</v>
       </c>
       <c r="H38">
-        <v>1.8125588642003936e-001</v>
+        <v>.960469825911913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Table 1 and 2 updated with missing coded as no
</commit_message>
<xml_diff>
--- a/table1.xlsx
+++ b/table1.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audrey\Documents\nhanes_ses_sleep_crp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="270" windowWidth="11100" windowHeight="5325"/>
+    <workbookView xWindow="720" yWindow="270" windowWidth="11100" windowHeight="5330"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="table1">'table1'!$A$1:$J$34</definedName>
+    <definedName name="table1">table1!$A$1:$J$32</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="true"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
   <si>
     <t>Table</t>
   </si>
@@ -91,12 +96,6 @@
     <t>birth_control</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>N/A (Male)</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -118,9 +117,6 @@
     <t>obese</t>
   </si>
   <si>
-    <t>      0</t>
-  </si>
-  <si>
     <t>pir_cat</t>
   </si>
   <si>
@@ -178,22 +174,19 @@
     <t>0.2493</t>
   </si>
   <si>
-    <t>0.1119</t>
-  </si>
-  <si>
     <t>0.0029</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>0.3842</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,20 +216,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,33 +228,316 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="5" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="8" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -293,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -302,10 +566,10 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -313,7 +577,7 @@
         <v>2629</v>
       </c>
       <c r="C2">
-        <v>.12486114311188569</v>
+        <v>0.1248611431118857</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -322,22 +586,22 @@
         <v>502</v>
       </c>
       <c r="F2">
-        <v>.18507942308033346</v>
+        <v>0.18507942308033351</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>1185</v>
       </c>
       <c r="I2">
-        <v>.4898956146358516</v>
+        <v>0.48989561463585152</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -345,7 +609,7 @@
         <v>3135</v>
       </c>
       <c r="C3">
-        <v>.26255386707176337</v>
+        <v>0.26255386707176326</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -354,22 +618,22 @@
         <v>319</v>
       </c>
       <c r="F3">
-        <v>.0797996404560808</v>
+        <v>7.9799640456080803E-2</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H3">
         <v>1419</v>
       </c>
       <c r="I3">
-        <v>.495217650639752</v>
+        <v>0.49521765063975193</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -377,7 +641,7 @@
         <v>3840</v>
       </c>
       <c r="C4">
-        <v>.24490627733231402</v>
+        <v>0.24490627733231404</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -386,22 +650,22 @@
         <v>672</v>
       </c>
       <c r="F4">
-        <v>.15581981197122155</v>
+        <v>0.15581981197122155</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H4">
         <v>1830</v>
       </c>
       <c r="I4">
-        <v>.5244569490000929</v>
+        <v>0.52445694900009299</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -409,7 +673,7 @@
         <v>2059</v>
       </c>
       <c r="C5">
-        <v>.06598153257734969</v>
+        <v>6.5981532577349691E-2</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -418,22 +682,22 @@
         <v>356</v>
       </c>
       <c r="F5">
-        <v>.16169120180728133</v>
+        <v>0.16169120180728133</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H5">
         <v>841</v>
       </c>
       <c r="I5">
-        <v>.43136326543532655</v>
+        <v>0.43136326543532649</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -441,7 +705,7 @@
         <v>4382</v>
       </c>
       <c r="C6">
-        <v>.30169717990668726</v>
+        <v>0.30169717990668726</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -450,22 +714,22 @@
         <v>739</v>
       </c>
       <c r="F6">
-        <v>.14891291937343276</v>
+        <v>0.14891291937343276</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6">
         <v>2040</v>
       </c>
       <c r="I6">
-        <v>.5126616125361327</v>
+        <v>0.51266161253613241</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -473,7 +737,7 @@
         <v>8073</v>
       </c>
       <c r="C7">
-        <v>.5117627120635093</v>
+        <v>0.51176271206350932</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -482,22 +746,22 @@
         <v>1297</v>
       </c>
       <c r="F7">
-        <v>.1354983682157096</v>
+        <v>0.1354983682157096</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>3840</v>
       </c>
       <c r="I7">
-        <v>.523752820413486</v>
+        <v>0.52375282041348603</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -505,7 +769,7 @@
         <v>7999</v>
       </c>
       <c r="C8">
-        <v>.4882372879364906</v>
+        <v>0.48823728793649074</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -514,22 +778,22 @@
         <v>1296</v>
       </c>
       <c r="F8">
-        <v>.140672320312189</v>
+        <v>0.14067232031218899</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>3482</v>
       </c>
       <c r="I8">
-        <v>.48016432037236295</v>
+        <v>0.4801643203723629</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -537,7 +801,7 @@
         <v>2895</v>
       </c>
       <c r="C9">
-        <v>.08140105460711192</v>
+        <v>8.1401054607111903E-2</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -546,22 +810,22 @@
         <v>377</v>
       </c>
       <c r="F9">
-        <v>.12119582655744879</v>
+        <v>0.12119582655744877</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H9">
         <v>1166</v>
       </c>
       <c r="I9">
-        <v>.41280301368474204</v>
+        <v>0.41280301368474209</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -569,7 +833,7 @@
         <v>3295</v>
       </c>
       <c r="C10">
-        <v>.11339982690459612</v>
+        <v>0.1133998269045961</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -578,22 +842,22 @@
         <v>851</v>
       </c>
       <c r="F10">
-        <v>.263793461420665</v>
+        <v>0.26379346142066501</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H10">
         <v>1527</v>
       </c>
       <c r="I10">
-        <v>.4641894244684604</v>
+        <v>0.46418942446846034</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -601,7 +865,7 @@
         <v>7779</v>
       </c>
       <c r="C11">
-        <v>.6997905026376184</v>
+        <v>0.69979050263761855</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
@@ -610,22 +874,22 @@
         <v>987</v>
       </c>
       <c r="F11">
-        <v>.11557434011829944</v>
+        <v>0.11557434011829944</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H11">
         <v>3817</v>
       </c>
       <c r="I11">
-        <v>.529225081865937</v>
+        <v>0.52922508186593697</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -633,7 +897,7 @@
         <v>1371</v>
       </c>
       <c r="C12">
-        <v>.04431119017169008</v>
+        <v>4.4311190171690093E-2</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -642,22 +906,22 @@
         <v>246</v>
       </c>
       <c r="F12">
-        <v>.1624588145847037</v>
+        <v>0.16245881458470371</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H12">
         <v>519</v>
       </c>
       <c r="I12">
-        <v>.4167798661601008</v>
+        <v>0.41677986616010088</v>
       </c>
       <c r="J12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -665,7 +929,7 @@
         <v>732</v>
       </c>
       <c r="C13">
-        <v>.06109742567898335</v>
+        <v>6.1097425678983346E-2</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -674,22 +938,22 @@
         <v>132</v>
       </c>
       <c r="F13">
-        <v>.16659755285831082</v>
+        <v>0.16659755285831079</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H13">
         <v>293</v>
       </c>
       <c r="I13">
-        <v>.448551759142935</v>
+        <v>0.4485517591429351</v>
       </c>
       <c r="J13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -697,31 +961,31 @@
         <v>15548</v>
       </c>
       <c r="C14">
-        <v>.9568064635229603</v>
+        <v>0.95680646352296062</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14">
         <v>2525</v>
       </c>
       <c r="F14">
-        <v>.13947862971407476</v>
+        <v>0.13947862971407471</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H14">
         <v>7059</v>
       </c>
       <c r="I14">
-        <v>.49860230632532104</v>
+        <v>0.4986023063253211</v>
       </c>
       <c r="J14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -729,612 +993,548 @@
         <v>524</v>
       </c>
       <c r="C15">
-        <v>.043193536477039905</v>
+        <v>4.3193536477039905E-2</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>68</v>
       </c>
       <c r="F15">
-        <v>.10586304778593553</v>
+        <v>0.10586304778593553</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>263</v>
       </c>
       <c r="I15">
-        <v>.5880940858461586</v>
+        <v>0.58809408584615852</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>4191</v>
       </c>
       <c r="C16">
-        <v>.2668761193923869</v>
+        <v>0.26687611939238703</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E16">
         <v>840</v>
       </c>
       <c r="F16">
-        <v>.1867148477516125</v>
+        <v>0.18671484775161251</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H16">
         <v>2022</v>
       </c>
       <c r="I16">
-        <v>.5299426217271924</v>
+        <v>0.52994262172719242</v>
       </c>
       <c r="J16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>11881</v>
       </c>
       <c r="C17">
-        <v>.7331238806076127</v>
+        <v>0.73312388060761247</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17">
         <v>1753</v>
       </c>
       <c r="F17">
-        <v>.12031952446696824</v>
+        <v>0.12031952446696824</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H17">
         <v>5300</v>
       </c>
       <c r="I17">
-        <v>.4924662840631326</v>
+        <v>0.49246628406313242</v>
       </c>
       <c r="J17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>15806</v>
       </c>
       <c r="C18">
-        <v>.9793049160211545</v>
+        <v>0.97930491602115488</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18">
         <v>2561</v>
       </c>
       <c r="F18">
-        <v>.13899455109226447</v>
+        <v>0.13899455109226444</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H18">
         <v>7158</v>
       </c>
       <c r="I18">
-        <v>.49925057241543896</v>
+        <v>0.49925057241543902</v>
       </c>
       <c r="J18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>266</v>
       </c>
       <c r="C19">
-        <v>.02069508397884525</v>
+        <v>2.0695083978845247E-2</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E19">
         <v>32</v>
       </c>
       <c r="F19">
-        <v>.0922032459515263</v>
+        <v>9.2203245951526319E-2</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H19">
         <v>164</v>
       </c>
       <c r="I19">
-        <v>.6547178499619064</v>
+        <v>0.65471784996190641</v>
       </c>
       <c r="J19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>10262</v>
       </c>
       <c r="C20">
-        <v>.6587112722226114</v>
+        <v>0.65871127222261139</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20">
         <v>1499</v>
       </c>
       <c r="F20">
-        <v>.1261754722221648</v>
+        <v>0.12617547222216483</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H20">
         <v>4702</v>
       </c>
       <c r="I20">
-        <v>.5072758279664283</v>
+        <v>0.50727582796642812</v>
       </c>
       <c r="J20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21">
         <v>5810</v>
       </c>
       <c r="C21">
-        <v>.3412887277773887</v>
+        <v>0.34128872777738872</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21">
         <v>1094</v>
       </c>
       <c r="F21">
-        <v>.1608998184941224</v>
+        <v>0.16089981849412249</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H21">
         <v>2620</v>
       </c>
       <c r="I21">
-        <v>.49319278243276726</v>
+        <v>0.49319278243276737</v>
       </c>
       <c r="J21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22">
-        <v>4442</v>
+        <v>7851</v>
       </c>
       <c r="C22">
-        <v>.3236744170748077</v>
+        <v>0.48286906137994334</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
       </c>
       <c r="E22">
-        <v>695</v>
+        <v>1289</v>
       </c>
       <c r="F22">
-        <v>.13479304388939517</v>
+        <v>0.14124217143313544</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22">
-        <v>3270</v>
+        <v>4458</v>
       </c>
       <c r="I22">
-        <v>.7692280837800479</v>
+        <v>0.63393402721978498</v>
       </c>
       <c r="J22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23">
-        <v>3409</v>
+        <v>8221</v>
       </c>
       <c r="C23">
-        <v>.15919464430513572</v>
+        <v>0.51713093862005666</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23">
-        <v>594</v>
+        <v>1304</v>
       </c>
       <c r="F23">
-        <v>.15434045425639598</v>
+        <v>0.13502321735951539</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23">
-        <v>1188</v>
+        <v>2864</v>
       </c>
       <c r="I23">
-        <v>.35881286903998816</v>
+        <v>0.37968712037296626</v>
       </c>
       <c r="J23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>8221</v>
+        <v>4316</v>
       </c>
       <c r="C24">
-        <v>.5171309386200567</v>
+        <v>0.18972914844892763</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E24">
-        <v>1304</v>
+        <v>839</v>
       </c>
       <c r="F24">
-        <v>.13502321735951536</v>
+        <v>0.18722574215352153</v>
       </c>
       <c r="G24" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H24">
-        <v>2864</v>
+        <v>1778</v>
       </c>
       <c r="I24">
-        <v>.3796871203729662</v>
+        <v>0.45477657312446518</v>
       </c>
       <c r="J24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>3962</v>
+      </c>
+      <c r="C25">
+        <v>0.18997926591229705</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <v>683</v>
+      </c>
+      <c r="F25">
+        <v>0.16913248837822439</v>
+      </c>
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25">
+        <v>1794</v>
+      </c>
+      <c r="I25">
+        <v>0.50744425187901243</v>
+      </c>
+      <c r="J25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>7794</v>
+      </c>
+      <c r="C26">
+        <v>0.62029158563877551</v>
+      </c>
+      <c r="D26" t="s">
         <v>34</v>
       </c>
-      <c r="B25">
-        <v>4316</v>
-      </c>
-      <c r="C25">
-        <v>.1897291484489276</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E26">
+        <v>1071</v>
+      </c>
+      <c r="F26">
+        <v>0.11349193345817842</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26">
+        <v>3750</v>
+      </c>
+      <c r="I26">
+        <v>0.51553301373273619</v>
+      </c>
+      <c r="J26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="E25">
-        <v>839</v>
-      </c>
-      <c r="F25">
-        <v>.1872257421535215</v>
-      </c>
-      <c r="G25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25">
-        <v>1778</v>
-      </c>
-      <c r="I25">
-        <v>.45477657312446507</v>
-      </c>
-      <c r="J25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26">
-        <v>3962</v>
-      </c>
-      <c r="C26">
-        <v>.18997926591229702</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B27">
+        <v>8741</v>
+      </c>
+      <c r="C27">
+        <v>0.49753098650550087</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27">
+        <v>1143</v>
+      </c>
+      <c r="F27">
+        <v>0.10819496651045324</v>
+      </c>
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>7322</v>
+      </c>
+      <c r="C28">
+        <v>0.50246901349449935</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>1448</v>
+      </c>
+      <c r="F28">
+        <v>0.16740678517893595</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="E26">
-        <v>683</v>
-      </c>
-      <c r="F26">
-        <v>.1691324883782244</v>
-      </c>
-      <c r="G26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26">
-        <v>1794</v>
-      </c>
-      <c r="I26">
-        <v>.5074442518790123</v>
-      </c>
-      <c r="J26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27">
-        <v>7794</v>
-      </c>
-      <c r="C27">
-        <v>.6202915856387755</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B29">
+        <v>13460</v>
+      </c>
+      <c r="C29">
+        <v>0.86197470541915644</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29">
+        <v>5862</v>
+      </c>
+      <c r="I29">
+        <v>0.48516092861343774</v>
+      </c>
+      <c r="J29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>2593</v>
+      </c>
+      <c r="C30">
+        <v>0.13802529458084364</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30">
+        <v>1448</v>
+      </c>
+      <c r="I30">
+        <v>0.60964505598207475</v>
+      </c>
+      <c r="J30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="E27">
-        <v>1071</v>
-      </c>
-      <c r="F27">
-        <v>.1134919334581784</v>
-      </c>
-      <c r="G27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27">
-        <v>3750</v>
-      </c>
-      <c r="I27">
-        <v>.5155330137327362</v>
-      </c>
-      <c r="J27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28">
-        <v>8741</v>
-      </c>
-      <c r="C28">
-        <v>.4975309865055008</v>
-      </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28">
-        <v>1143</v>
-      </c>
-      <c r="F28">
-        <v>.10819496651045324</v>
-      </c>
-      <c r="G28" t="s">
-        <v>44</v>
-      </c>
-      <c r="J28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29">
-        <v>7322</v>
-      </c>
-      <c r="C29">
-        <v>.5024690134944994</v>
-      </c>
-      <c r="D29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29">
-        <v>1448</v>
-      </c>
-      <c r="F29">
-        <v>.1674067851789359</v>
-      </c>
-      <c r="G29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30">
-        <v>13460</v>
-      </c>
-      <c r="C30">
-        <v>.8619747054191564</v>
-      </c>
-      <c r="D30" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" t="s">
-        <v>55</v>
-      </c>
-      <c r="H30">
-        <v>5862</v>
-      </c>
-      <c r="I30">
-        <v>.48516092861343796</v>
-      </c>
-      <c r="J30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>39</v>
-      </c>
       <c r="B31">
-        <v>2593</v>
+        <v>15271</v>
       </c>
       <c r="C31">
-        <v>.13802529458084364</v>
+        <v>0.94257714535313109</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="E31">
+        <v>2399</v>
+      </c>
+      <c r="F31">
+        <v>0.13344442768370821</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H31">
-        <v>1448</v>
+        <v>6561</v>
       </c>
       <c r="I31">
-        <v>.6096450559820747</v>
+        <v>0.47455758973325929</v>
       </c>
       <c r="J31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B32">
-        <v>612</v>
+        <v>801</v>
       </c>
       <c r="C32">
-        <v>.04055348062536871</v>
+        <v>5.7422854646869123E-2</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E32">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="F32">
-        <v>.21491655551873742</v>
+        <v>0.21314409695001449</v>
       </c>
       <c r="G32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H32">
-        <v>548</v>
+        <v>761</v>
       </c>
       <c r="I32">
-        <v>.9046874261574475</v>
+        <v>0.96046982591191332</v>
       </c>
       <c r="J32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33">
-        <v>14659</v>
-      </c>
-      <c r="C33">
-        <v>.9020236647277617</v>
-      </c>
-      <c r="D33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33">
-        <v>2246</v>
-      </c>
-      <c r="F33">
-        <v>.12978994006035618</v>
-      </c>
-      <c r="G33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33">
-        <v>6013</v>
-      </c>
-      <c r="I33">
-        <v>.4552273107625041</v>
-      </c>
-      <c r="J33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34">
-        <v>801</v>
-      </c>
-      <c r="C34">
-        <v>.057422854646869116</v>
-      </c>
-      <c r="D34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34">
-        <v>194</v>
-      </c>
-      <c r="F34">
-        <v>.21314409695001446</v>
-      </c>
-      <c r="G34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34">
-        <v>761</v>
-      </c>
-      <c r="I34">
-        <v>.960469825911913</v>
-      </c>
-      <c r="J34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>